<commit_message>
fixed unit in Readme
</commit_message>
<xml_diff>
--- a/Data/Exp 3 Column Experiment ColEx Data/CDOM/24-10-30_TMP_ColEx_CDOM/7_Spectral indices/R_SpectralIndices_ReadMe.xlsx
+++ b/Data/Exp 3 Column Experiment ColEx Data/CDOM/24-10-30_TMP_ColEx_CDOM/7_Spectral indices/R_SpectralIndices_ReadMe.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimj704/Github/CDOM_EEMs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimj704/Github/tempest_ionic_strength/Data/Exp 3 Column Experiment ColEx Data/CDOM/24-10-30_TMP_ColEx_CDOM/7_Spectral indices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0714F34F-821B-3C47-8E86-10BDEC646D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CED227-D7C5-1A45-8CE9-D4BCB8EE8D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="800" windowWidth="28040" windowHeight="17120" xr2:uid="{6314DAA8-72C2-BD44-9DCA-B5E505800B13}"/>
   </bookViews>
@@ -170,9 +170,6 @@
     <t>sum(435:480)/sum(300:345)</t>
   </si>
   <si>
-    <t>[L mgC^(-1)m(-1)]</t>
-  </si>
-  <si>
     <t>Hansen et al., 2016</t>
   </si>
   <si>
@@ -333,6 +330,9 @@
   </si>
   <si>
     <t>Zsolnay 1999</t>
+  </si>
+  <si>
+    <t>[L mgC^(-1)m^(-1)]</t>
   </si>
 </sst>
 </file>
@@ -553,18 +553,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -579,23 +579,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
@@ -603,30 +588,44 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -963,46 +962,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D61A842-7AC1-BC49-8ED3-35828E77E2D7}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="108" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="15"/>
-    <col min="2" max="2" width="57.1640625" style="15" customWidth="1"/>
-    <col min="3" max="3" width="30.5" style="15" customWidth="1"/>
-    <col min="4" max="4" width="60.6640625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="15" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="10"/>
+    <col min="2" max="2" width="57.1640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="30.5" style="10" customWidth="1"/>
+    <col min="4" max="4" width="60.6640625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
-        <v>55</v>
+      <c r="A1" s="28" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1016,10 +1015,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1033,10 +1032,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1050,10 +1049,10 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1067,10 +1066,10 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1084,16 +1083,16 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="22">
+      <c r="A8" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="17">
         <v>390</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="17">
         <v>509</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -1101,16 +1100,16 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9" s="22">
+      <c r="A9" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="17">
         <v>455</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="17">
         <v>521</v>
       </c>
       <c r="E9" s="5" t="s">
@@ -1118,16 +1117,16 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10" s="22">
+      <c r="A10" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="17">
         <v>280</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="17">
         <v>370</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -1135,62 +1134,62 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B12" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B13" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="s">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B14" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="23" t="s">
-        <v>45</v>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="18" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="16" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="3">
@@ -1202,25 +1201,25 @@
       <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="21" t="s">
+      <c r="A16" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="19"/>
+      <c r="E16" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="C16" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="23" t="s">
-        <v>94</v>
-      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="3">
@@ -1230,245 +1229,245 @@
         <v>43</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>95</v>
+      <c r="A18" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>94</v>
       </c>
       <c r="C18" s="3">
         <v>254</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="21" t="s">
+      <c r="A19" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="16" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="3">
         <v>310</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="C20" s="35" t="s">
+      <c r="A20" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="16" t="s">
         <v>96</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>95</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="21" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="7">
         <v>310</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="8"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="28"/>
-      <c r="B22" s="28"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B23" s="28"/>
+      <c r="A23" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="22"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="32" t="s">
+    </row>
+    <row r="25" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="30"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="34"/>
+    </row>
+    <row r="26" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="30"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="34"/>
+    </row>
+    <row r="27" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="30"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="34"/>
+    </row>
+    <row r="28" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="C28" s="30"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="34"/>
+    </row>
+    <row r="29" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" s="30"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="34"/>
+    </row>
+    <row r="30" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" s="30"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="34"/>
+    </row>
+    <row r="31" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="30"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="34"/>
+    </row>
+    <row r="32" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="30"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="34"/>
+    </row>
+    <row r="33" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" s="30"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="34"/>
+    </row>
+    <row r="34" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B25" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="12"/>
-    </row>
-    <row r="26" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="12"/>
-    </row>
-    <row r="27" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="12"/>
-    </row>
-    <row r="28" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="12"/>
-    </row>
-    <row r="29" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="12"/>
-    </row>
-    <row r="30" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="12"/>
-    </row>
-    <row r="31" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="B31" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="C31" s="9"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="12"/>
-    </row>
-    <row r="32" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="B32" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="12"/>
-    </row>
-    <row r="33" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="B33" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="12"/>
-    </row>
-    <row r="34" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="20" t="s">
+      <c r="D34" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="34"/>
+    </row>
+    <row r="35" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C34" s="1" t="s">
+      <c r="B35" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34" s="12"/>
-    </row>
-    <row r="35" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B35" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C35" s="1" t="s">
+      <c r="D35" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" s="34"/>
+    </row>
+    <row r="36" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D35" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="E35" s="12"/>
-    </row>
-    <row r="36" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B36" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="D36" s="27" t="s">
+      <c r="D36" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="14"/>
+      <c r="E36" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>